<commit_message>
conceptual_models.xlsx file created: it collects all working concepts. Placed in default folder
</commit_message>
<xml_diff>
--- a/default/1_sut_multi_year/concept.xlsx
+++ b/default/1_sut_multi_year/concept.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\4_multi_year_simple\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\1_sut_multi_year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0575AFA8-7847-42B0-A328-F7C2A25E7E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8617B0D5-0BE6-4802-A796-670EF7EB252E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{0A3BC822-FD99-4F89-AC4E-FBD077FFAF78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0A3BC822-FD99-4F89-AC4E-FBD077FFAF78}"/>
   </bookViews>
   <sheets>
     <sheet name="multi-year" sheetId="6" r:id="rId1"/>
@@ -695,18 +695,18 @@
   <dimension ref="A1:AE31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="6.54296875" customWidth="1"/>
+    <col min="1" max="4" width="6.5703125" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.54296875" customWidth="1"/>
-    <col min="7" max="47" width="6.1796875" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="47" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -756,7 +756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -769,14 +769,14 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>37</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -790,7 +790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>4</v>
       </c>
@@ -812,12 +812,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
         <v>21</v>
       </c>
@@ -831,7 +831,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -883,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>28</v>
       </c>
@@ -945,7 +945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>3</v>
       </c>
@@ -993,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>6</v>
       </c>
@@ -1040,12 +1040,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>38</v>
       </c>
@@ -1065,12 +1065,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>172.8</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1135,12 +1135,12 @@
         <v>207.36</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1202,12 +1202,12 @@
         <v>4147.2000000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="M30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="M31" s="14">
         <v>1</v>
       </c>

</xml_diff>